<commit_message>
Adding input csv processing functionality
</commit_message>
<xml_diff>
--- a/documentation/INPUT/Site to Command.xlsx
+++ b/documentation/INPUT/Site to Command.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10523"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhutto\Desktop\DEPLOY SOLUTION\INPUT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dpheasan/Documents/BlueMetal/clients/FedEx/PsGenericAppInstaller/documentation/INPUT/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D4E7F1EE-081C-4247-9096-C6FB0E9BADF5}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="7030"/>
+    <workbookView xWindow="0" yWindow="3520" windowWidth="26680" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
-  <si>
-    <t>Site</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Package Location</t>
   </si>
@@ -35,57 +33,27 @@
     <t>Execution Command Line</t>
   </si>
   <si>
-    <t>CAS</t>
-  </si>
-  <si>
     <t>\\c0005280.corp.ds.fedex.com\source$\adaptiva\</t>
   </si>
   <si>
     <t>msiexec /I AdaptivaP2PClientInstaller.msi /q SERVERNAME=c0004513.corp.ds.fedex.com SOURCEUNCPATH=\\c0005280.corp.ds.fedex.com\source$\adaptiva\AdaptivaClientSetup.exe WAITFORCOMPLETION=1  </t>
   </si>
   <si>
-    <t>FP1</t>
-  </si>
-  <si>
     <t>msiexec /I AdaptivaP2PClientInstaller.msi /q SERVERNAME=c0004517.corp.ds.fedex.com SOURCEUNCPATH=\\c0005280.corp.ds.fedex.com\source$\adaptiva\AdaptivaClientSetup.exe WAITFORCOMPLETION=1  </t>
   </si>
   <si>
-    <t>FP2</t>
-  </si>
-  <si>
     <t>msiexec /I AdaptivaP2PClientInstaller.msi /q SERVERNAME=c0004515.corp.ds.fedex.com SOURCEUNCPATH=\\c0005280.corp.ds.fedex.com\source$\adaptiva\AdaptivaClientSetup.exe WAITFORCOMPLETION=1  </t>
   </si>
   <si>
-    <t>FP3</t>
-  </si>
-  <si>
     <t>msiexec /I AdaptivaP2PClientInstaller.msi /q SERVERNAME=pwn04516.corp.ds.fedex.com SOURCEUNCPATH=\\c0005280.corp.ds.fedex.com\source$\adaptiva\AdaptivaClientSetup.exe WAITFORCOMPLETION=1  </t>
   </si>
   <si>
-    <t>FP4</t>
-  </si>
-  <si>
     <t>msiexec /I AdaptivaP2PClientInstaller.msi /q SERVERNAME=pwn58025.corp.ds.fedex.com SOURCEUNCPATH=\\c0005280.corp.ds.fedex.com\source$\adaptiva\AdaptivaClientSetup.exe WAITFORCOMPLETION=1  </t>
   </si>
   <si>
-    <t>FP5</t>
-  </si>
-  <si>
-    <t>msiexec /I AdaptivaP2PClientInstaller.msi /q SERVERNAME=pwn04520.corp.ds.fedex.com SOURCEUNCPATH=\\c0005280.corp.ds.fedex.com\source$\adaptiva\AdaptivaClientSetup.exe WAITFORCOMPLETION=1  </t>
-  </si>
-  <si>
-    <t>FP6</t>
-  </si>
-  <si>
-    <t>msiexec /I AdaptivaP2PClientInstaller.msi /q SERVERNAME=pwn58039.corp.ds.fedex.com SOURCEUNCPATH=\\c0005280.corp.ds.fedex.com\source$\adaptiva\AdaptivaClientSetup.exe WAITFORCOMPLETION=1  </t>
-  </si>
-  <si>
     <t>Installed Logfile Location</t>
   </si>
   <si>
-    <t>TBD?</t>
-  </si>
-  <si>
     <t>Client Local Path</t>
   </si>
   <si>
@@ -98,17 +66,29 @@
     <t>Logfile Regex</t>
   </si>
   <si>
-    <t xml:space="preserve">$NULL </t>
-  </si>
-  <si>
-    <t>VALUE</t>
+    <t>Site ID</t>
+  </si>
+  <si>
+    <t>Site1</t>
+  </si>
+  <si>
+    <t>Site2</t>
+  </si>
+  <si>
+    <t>Site3</t>
+  </si>
+  <si>
+    <t>Site4</t>
+  </si>
+  <si>
+    <t>Site5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -452,197 +432,135 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.81640625" customWidth="1"/>
-    <col min="2" max="2" width="20.81640625" customWidth="1"/>
-    <col min="3" max="3" width="24.1796875" customWidth="1"/>
-    <col min="4" max="4" width="35.7265625" customWidth="1"/>
-    <col min="5" max="5" width="35.453125" customWidth="1"/>
-    <col min="6" max="6" width="57.81640625" customWidth="1"/>
+    <col min="1" max="1" width="26.83203125" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="157.6640625" customWidth="1"/>
+    <col min="6" max="6" width="57.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16">
+      <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="E2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16">
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16">
+      <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="D6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="F6" t="s">
         <v>9</v>
       </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:6" ht="16">
+      <c r="A7" s="2"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" ht="16">
+      <c r="A8" s="2"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="D5" r:id="rId4"/>
-    <hyperlink ref="D6" r:id="rId5"/>
-    <hyperlink ref="D7" r:id="rId6"/>
-    <hyperlink ref="D8" r:id="rId7"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>